<commit_message>
LPF with VR test
</commit_message>
<xml_diff>
--- a/pico-synth-sound/filter.xlsx
+++ b/pico-synth-sound/filter.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e6113d96ddfeabfd/22_Development/34_pico_synth/pico-synth-sound/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="11_AD4D066CA252ABDACC10483C11D3D62073EEDF4E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DB8ADE5-5C70-44C9-A14A-23500E6E4E03}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_AD4D066CA252ABDACC10483C11D3D62073EEDF4E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF4F03E4-65E9-48CD-9DF3-1313E21AC22E}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>sampling_rate</t>
     <phoneticPr fontId="1"/>
@@ -83,6 +83,26 @@
   </si>
   <si>
     <t>b_2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b_0_a_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b_1_a_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>b_2_a_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a_1_a_0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>a_2_a_0</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -411,10 +431,13 @@
   <dimension ref="A1:K301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75"/>
+  <cols>
+    <col min="10" max="10" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -442,7 +465,7 @@
         <v>3</v>
       </c>
       <c r="K2">
-        <v>4000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -457,7 +480,7 @@
         <v>4</v>
       </c>
       <c r="K3">
-        <v>1</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -482,7 +505,7 @@
       </c>
       <c r="K5">
         <f>2*PI()*K2/K1</f>
-        <v>0.62831853071795862</v>
+        <v>0.31415926535897931</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -498,7 +521,7 @@
       </c>
       <c r="K6">
         <f>SIN(K5)/(2*K3)</f>
-        <v>0.29389262614623657</v>
+        <v>0.10300566479164913</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -514,7 +537,7 @@
       </c>
       <c r="K7">
         <f>1+K6</f>
-        <v>1.2938926261462367</v>
+        <v>1.1030056647916491</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -530,7 +553,7 @@
       </c>
       <c r="K8">
         <f>-2*COS(K5)</f>
-        <v>-1.6180339887498949</v>
+        <v>-1.9021130325903071</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -546,7 +569,7 @@
       </c>
       <c r="K9">
         <f>1-K6</f>
-        <v>0.70610737385376343</v>
+        <v>0.89699433520835092</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -562,7 +585,7 @@
       </c>
       <c r="K10">
         <f>(1-COS(K5))/2</f>
-        <v>9.5491502812526274E-2</v>
+        <v>2.4471741852423234E-2</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -578,7 +601,7 @@
       </c>
       <c r="K11">
         <f>1-COS(K5)</f>
-        <v>0.19098300562505255</v>
+        <v>4.8943483704846469E-2</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -594,7 +617,7 @@
       </c>
       <c r="K12">
         <f>(1-COS(K5))/2</f>
-        <v>9.5491502812526274E-2</v>
+        <v>2.4471741852423234E-2</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -605,6 +628,13 @@
         <f t="shared" si="0"/>
         <v>0.18849555921538758</v>
       </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="K13">
+        <f>K10/K7</f>
+        <v>2.2186415386221788E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14">
@@ -614,6 +644,13 @@
         <f t="shared" si="0"/>
         <v>0.20420352248333654</v>
       </c>
+      <c r="J14" t="s">
+        <v>13</v>
+      </c>
+      <c r="K14">
+        <f>K11/K7</f>
+        <v>4.4372830772443576E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15">
@@ -623,6 +660,13 @@
         <f t="shared" si="0"/>
         <v>0.2199114857512855</v>
       </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <f>K12/K7</f>
+        <v>2.2186415386221788E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16">
@@ -632,8 +676,15 @@
         <f t="shared" si="0"/>
         <v>0.23561944901923448</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="J16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16">
+        <f>K8/K7</f>
+        <v>-1.7244816534551564</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17">
         <v>1600</v>
       </c>
@@ -641,8 +692,15 @@
         <f t="shared" si="0"/>
         <v>0.25132741228718347</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="J17" t="s">
+        <v>16</v>
+      </c>
+      <c r="K17">
+        <f>K9/K7</f>
+        <v>0.81322731500004364</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18">
         <v>1700</v>
       </c>
@@ -651,7 +709,7 @@
         <v>0.2670353755551324</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:11">
       <c r="A19">
         <v>1800</v>
       </c>
@@ -660,7 +718,7 @@
         <v>0.28274333882308139</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:11">
       <c r="A20">
         <v>1900</v>
       </c>
@@ -669,7 +727,7 @@
         <v>0.29845130209103038</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:11">
       <c r="A21">
         <v>2000</v>
       </c>
@@ -678,7 +736,7 @@
         <v>0.31415926535897931</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:11">
       <c r="A22">
         <v>2100</v>
       </c>
@@ -687,7 +745,7 @@
         <v>0.3298672286269283</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:11">
       <c r="A23">
         <v>2200</v>
       </c>
@@ -696,7 +754,7 @@
         <v>0.34557519189487723</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:11">
       <c r="A24">
         <v>2300</v>
       </c>
@@ -705,7 +763,7 @@
         <v>0.36128315516282616</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:11">
       <c r="A25">
         <v>2400</v>
       </c>
@@ -714,7 +772,7 @@
         <v>0.37699111843077515</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:11">
       <c r="A26">
         <v>2500</v>
       </c>
@@ -723,7 +781,7 @@
         <v>0.39269908169872414</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:11">
       <c r="A27">
         <v>2600</v>
       </c>
@@ -732,7 +790,7 @@
         <v>0.40840704496667307</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:11">
       <c r="A28">
         <v>2700</v>
       </c>
@@ -741,7 +799,7 @@
         <v>0.42411500823462212</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:11">
       <c r="A29">
         <v>2800</v>
       </c>
@@ -750,7 +808,7 @@
         <v>0.43982297150257099</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:11">
       <c r="A30">
         <v>2900</v>
       </c>
@@ -759,7 +817,7 @@
         <v>0.45553093477051998</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:11">
       <c r="A31">
         <v>3000</v>
       </c>
@@ -768,7 +826,7 @@
         <v>0.47123889803846897</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:11">
       <c r="A32">
         <v>3100</v>
       </c>
@@ -3201,5 +3259,6 @@
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>